<commit_message>
Tarefa 2 dos 10 testes de mesa e mudançan nos exercícios 9,10,11,12 e 14
</commit_message>
<xml_diff>
--- a/Tarefa 1/TesteDeMesa.xlsx
+++ b/Tarefa 1/TesteDeMesa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André\Desktop\Fatec\Banco de Dados\2º Semestre\Linguagem de programação 1\Tarefa 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CC3557-352A-45F7-8E02-2274C578565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F82A7C-4958-4803-A4F0-F08BAD436742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{342F45EC-93DB-4454-8543-AC7D7920A6FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Teste de mesa 1</t>
   </si>
@@ -183,6 +183,135 @@
   </si>
   <si>
     <t>Imprime totalEleitores, percentualValidos, percentualBranco, percentualNulos</t>
+  </si>
+  <si>
+    <t>Teste de mesa 6</t>
+  </si>
+  <si>
+    <t>Digite seu salário</t>
+  </si>
+  <si>
+    <t>Digite o percentual de reajuste</t>
+  </si>
+  <si>
+    <t>Conta do salário x reajuste</t>
+  </si>
+  <si>
+    <t>Imprime salarioReajustado</t>
+  </si>
+  <si>
+    <t>salario</t>
+  </si>
+  <si>
+    <t>reajuste</t>
+  </si>
+  <si>
+    <t>salarioReajustado</t>
+  </si>
+  <si>
+    <t>Teste de mesa 7</t>
+  </si>
+  <si>
+    <t>custo</t>
+  </si>
+  <si>
+    <t>custoTotal</t>
+  </si>
+  <si>
+    <t>Digite o valor do carro</t>
+  </si>
+  <si>
+    <t>Imprime custoTotal</t>
+  </si>
+  <si>
+    <t>Conta do custoTotal</t>
+  </si>
+  <si>
+    <t>Teste de mesa 8</t>
+  </si>
+  <si>
+    <t>valuePerCar</t>
+  </si>
+  <si>
+    <t>salesCars</t>
+  </si>
+  <si>
+    <t>salesTotals</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>totalSalary</t>
+  </si>
+  <si>
+    <t>Digite seu salário fixo</t>
+  </si>
+  <si>
+    <t>Digite a quantidade de carros vendidos</t>
+  </si>
+  <si>
+    <t>Digite o total das vendas</t>
+  </si>
+  <si>
+    <t>Digite o valor a receber por carro vendido</t>
+  </si>
+  <si>
+    <t>Conta do totalSalary</t>
+  </si>
+  <si>
+    <t>Imprime name e totalSalary</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>"André Luiz"</t>
+  </si>
+  <si>
+    <t>Teste de mesa 9</t>
+  </si>
+  <si>
+    <t>Instânciando objeto com o construtor name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instânciando objeto Exercicio12 com o construtor grausCelsius </t>
+  </si>
+  <si>
+    <t>grausCelsius</t>
+  </si>
+  <si>
+    <t>transformaGrausFahren</t>
+  </si>
+  <si>
+    <t>Imprime grausCelsius e chama método transformaGrausFahren</t>
+  </si>
+  <si>
+    <t>Teste de mesa 10</t>
+  </si>
+  <si>
+    <t>Instânciando objeto Exercicio13</t>
+  </si>
+  <si>
+    <t>Chama método maiorOuMenor</t>
+  </si>
+  <si>
+    <t>Digite um número</t>
+  </si>
+  <si>
+    <t>Imprime se um número é maior que 10</t>
+  </si>
+  <si>
+    <t>Imprime se um número é menor que 10</t>
+  </si>
+  <si>
+    <t>Condição</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -303,27 +432,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -337,12 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,6 +459,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,18 +801,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81D61DA-AC68-48DF-8102-2EF29293A6F5}">
-  <dimension ref="B2:J41"/>
+  <dimension ref="B2:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="40.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -685,639 +820,639 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>10</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>20</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="B7" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>20</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>20</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>10</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="12">
+      <c r="B9" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>20</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>10</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+      <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
+      <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
+      <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>20</v>
       </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
+      <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>20</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>10</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
+      <c r="B20" s="7">
         <v>3</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>20</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>10</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
+      <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>20</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>10</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>200</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="12">
+      <c r="B25" s="7">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>23</v>
       </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="3">
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
+      <c r="B26" s="7">
         <v>2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>23</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>4</v>
       </c>
-      <c r="F26" s="3">
-        <v>0</v>
-      </c>
-      <c r="G26" s="3">
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="12">
+      <c r="B27" s="7">
         <v>3</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>23</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>4</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>20</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="12">
+      <c r="B28" s="7">
         <v>4</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>23</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>4</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>20</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>8535</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="12">
+      <c r="B29" s="7">
         <v>5</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>23</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>4</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>20</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>8535</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="H32" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="15" t="s">
+      <c r="J32" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="11">
+      <c r="B33" s="6">
         <v>1</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="4">
         <v>1000</v>
       </c>
-      <c r="E33" s="9">
-        <v>0</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0</v>
-      </c>
-      <c r="G33" s="9">
-        <v>0</v>
-      </c>
-      <c r="H33" s="10">
-        <v>0</v>
-      </c>
-      <c r="I33" s="10">
-        <v>0</v>
-      </c>
-      <c r="J33" s="10">
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="12">
+      <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="5">
         <v>1000</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="5">
         <v>500</v>
       </c>
-      <c r="F34" s="10">
-        <v>0</v>
-      </c>
-      <c r="G34" s="10">
-        <v>0</v>
-      </c>
-      <c r="H34" s="10">
-        <v>0</v>
-      </c>
-      <c r="I34" s="10">
-        <v>0</v>
-      </c>
-      <c r="J34" s="10">
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="12">
+      <c r="B35" s="7">
         <v>3</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="5">
         <v>1000</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="5">
         <v>500</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="5">
         <v>200</v>
       </c>
-      <c r="G35" s="10">
-        <v>0</v>
-      </c>
-      <c r="H35" s="10">
-        <v>0</v>
-      </c>
-      <c r="I35" s="10">
-        <v>0</v>
-      </c>
-      <c r="J35" s="10">
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="12">
+      <c r="B36" s="7">
         <v>4</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="5">
         <v>1000</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="5">
         <v>500</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="5">
         <v>200</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="5">
         <v>300</v>
       </c>
-      <c r="H36" s="10">
-        <v>0</v>
-      </c>
-      <c r="I36" s="10">
-        <v>0</v>
-      </c>
-      <c r="J36" s="10">
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="12">
+      <c r="B37" s="7">
         <v>5</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="5">
         <v>1000</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="5">
         <v>500</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="5">
         <v>200</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="5">
         <v>300</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="5">
         <v>30</v>
       </c>
-      <c r="I37" s="10">
-        <v>0</v>
-      </c>
-      <c r="J37" s="10">
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="12">
+      <c r="B38" s="7">
         <v>6</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="5">
         <v>1000</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="5">
         <v>500</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="5">
         <v>200</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="5">
         <v>300</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38" s="5">
         <v>30</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="5">
         <v>50</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="12">
+      <c r="B39" s="7">
         <v>7</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="5">
         <v>1000</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="5">
         <v>500</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="5">
         <v>200</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="5">
         <v>300</v>
       </c>
-      <c r="H39" s="10">
+      <c r="H39" s="5">
         <v>30</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I39" s="5">
         <v>50</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="5">
         <v>20</v>
       </c>
     </row>
@@ -1325,58 +1460,587 @@
       <c r="B40" s="13">
         <v>8</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="9">
         <v>1000</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="9">
         <v>500</v>
       </c>
-      <c r="F40" s="16">
+      <c r="F40" s="9">
         <v>200</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="9">
         <v>300</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H40" s="9">
         <v>30</v>
       </c>
-      <c r="I40" s="16">
+      <c r="I40" s="9">
         <v>50</v>
       </c>
-      <c r="J40" s="16">
+      <c r="J40" s="9">
         <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="17">
+      <c r="C41" s="12"/>
+      <c r="D41" s="10">
         <v>1000</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="10">
         <v>500</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="10">
         <v>200</v>
       </c>
-      <c r="G41" s="17">
+      <c r="G41" s="10">
         <v>300</v>
       </c>
-      <c r="H41" s="17">
+      <c r="H41" s="10">
         <v>30</v>
       </c>
-      <c r="I41" s="17">
+      <c r="I41" s="10">
         <v>50</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="10">
         <v>20</v>
       </c>
     </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="7">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1741</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="7">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1741</v>
+      </c>
+      <c r="E46" s="2">
+        <v>4</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="7">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1741</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1810.64</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="7">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1741</v>
+      </c>
+      <c r="E48" s="2">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1810.64</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="16"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="7">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="2">
+        <v>22000</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="7">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="2">
+        <v>22000</v>
+      </c>
+      <c r="E53" s="2">
+        <v>38060</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="7">
+        <v>3</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="2">
+        <v>22000</v>
+      </c>
+      <c r="E54" s="2">
+        <v>38060</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="6">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="7">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="5">
+        <v>0</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="7">
+        <v>3</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="5">
+        <v>0</v>
+      </c>
+      <c r="E60" s="5">
+        <v>10</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H60" s="5">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="7">
+        <v>4</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5">
+        <v>10</v>
+      </c>
+      <c r="F61" s="5">
+        <v>500</v>
+      </c>
+      <c r="G61" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="7">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" s="5">
+        <v>200</v>
+      </c>
+      <c r="E62" s="5">
+        <v>10</v>
+      </c>
+      <c r="F62" s="5">
+        <v>500</v>
+      </c>
+      <c r="G62" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H62" s="5">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="7">
+        <v>6</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="5">
+        <v>200</v>
+      </c>
+      <c r="E63" s="5">
+        <v>10</v>
+      </c>
+      <c r="F63" s="5">
+        <v>500</v>
+      </c>
+      <c r="G63" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H63" s="5">
+        <v>3766</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="7">
+        <v>7</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="5">
+        <v>200</v>
+      </c>
+      <c r="E64" s="5">
+        <v>10</v>
+      </c>
+      <c r="F64" s="5">
+        <v>500</v>
+      </c>
+      <c r="G64" s="5">
+        <v>1741</v>
+      </c>
+      <c r="H64" s="5">
+        <v>3766</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="16"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="7">
+        <v>1</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="7">
+        <v>33</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="7">
+        <v>2</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D69" s="7">
+        <v>33</v>
+      </c>
+      <c r="E69" s="7">
+        <v>91.4</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="16"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="7">
+        <v>1</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="7">
+        <v>0</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="7">
+        <v>2</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" s="7">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="7">
+        <v>3</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="7">
+        <v>4</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="7">
+        <v>5</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="7">
+        <v>0</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="19">
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B43:F43"/>
     <mergeCell ref="I40:I41"/>
     <mergeCell ref="J40:J41"/>
     <mergeCell ref="B31:J31"/>
@@ -1387,10 +2051,6 @@
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="G40:G41"/>
     <mergeCell ref="H40:H41"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B23:G23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>